<commit_message>
v2 pcb, code for pid, data for pid on bike
</commit_message>
<xml_diff>
--- a/calculating frequency of speed updates.xlsx
+++ b/calculating frequency of speed updates.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harri\Dropbox\2017-2018 Human Powered Vehicle\Electrical\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -59,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -189,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,26 +217,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,23 +252,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,11 +427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,11 +486,11 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
         <f>B2*1.6*1000/60/60</f>
-        <v>0.44444444444444448</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="D2" s="3">
         <v>2136</v>
@@ -540,14 +501,14 @@
       </c>
       <c r="F2" s="2">
         <f>C2/E2</f>
-        <v>0.20807324178110695</v>
+        <v>1.2484394506866419</v>
       </c>
       <c r="G2" s="1">
         <v>8</v>
       </c>
       <c r="H2" s="5">
         <f>F2*G2</f>
-        <v>1.6645859342488556</v>
+        <v>9.9875156054931349</v>
       </c>
       <c r="I2" s="1">
         <v>10</v>
@@ -557,11 +518,11 @@
       </c>
       <c r="K2" s="2">
         <f>C2/I2/J2</f>
-        <v>0.17777777777777778</v>
+        <v>1.0666666666666669</v>
       </c>
       <c r="L2" s="6">
         <f>C2/2*K2</f>
-        <v>3.9506172839506179E-2</v>
+        <v>1.4222222222222227</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -2539,7 +2500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2551,7 +2512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>